<commit_message>
Continued work on Cancellation logic for relationships.
</commit_message>
<xml_diff>
--- a/docs/Relationship CancelEdit.xlsx
+++ b/docs/Relationship CancelEdit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="20895" windowHeight="9660"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="20895" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -27,9 +27,6 @@
     <t>Association</t>
   </si>
   <si>
-    <t>Relationship</t>
-  </si>
-  <si>
     <t>Relationship Edited</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>1(FK) - 1</t>
   </si>
   <si>
-    <t>Child</t>
-  </si>
-  <si>
     <t>Added Child</t>
   </si>
   <si>
@@ -136,6 +130,12 @@
   </si>
   <si>
     <t>No Action</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Non-Owner</t>
   </si>
 </sst>
 </file>
@@ -864,40 +864,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,8 +1197,8 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1207,8 +1207,9 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="7" width="8.28515625" customWidth="1"/>
-    <col min="8" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="12" width="9.42578125" customWidth="1"/>
+    <col min="8" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" customWidth="1"/>
   </cols>
@@ -1218,11 +1219,11 @@
     </row>
     <row r="2" spans="1:15">
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
       <c r="L2" s="36"/>
       <c r="M2" s="35"/>
     </row>
@@ -1232,37 +1233,37 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="62"/>
+      <c r="F4" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="62"/>
+      <c r="H4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="57" t="s">
+      <c r="I4" s="62"/>
+      <c r="J4" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="62"/>
+      <c r="L4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="58"/>
-      <c r="L4" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="58"/>
+      <c r="M4" s="62"/>
       <c r="O4"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickTop="1">
       <c r="A5" s="12"/>
-      <c r="B5" s="63" t="s">
-        <v>16</v>
+      <c r="B5" s="53" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D5" s="37" t="str">
         <f>$B$14</f>
@@ -1278,20 +1279,20 @@
         <v>-A</v>
       </c>
       <c r="H5" s="39" t="str">
+        <f>B24</f>
+        <v>R + C</v>
+      </c>
+      <c r="I5" s="45" t="str">
+        <f>$B$21</f>
+        <v>-C</v>
+      </c>
+      <c r="J5" s="39" t="str">
         <f>B25</f>
         <v>A + C</v>
       </c>
-      <c r="I5" s="46" t="str">
+      <c r="K5" s="46" t="str">
         <f>$B$20</f>
         <v>-R</v>
-      </c>
-      <c r="J5" s="39" t="str">
-        <f>B24</f>
-        <v>R + C</v>
-      </c>
-      <c r="K5" s="45" t="str">
-        <f>$B$21</f>
-        <v>-C</v>
       </c>
       <c r="L5" s="40" t="str">
         <f>B26</f>
@@ -1304,9 +1305,9 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="A6" s="12"/>
-      <c r="B6" s="64"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="18" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D6" s="47" t="str">
         <f>$B$14</f>
@@ -1322,12 +1323,12 @@
         <f>$B$14</f>
         <v>C</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="30" t="str">
         <f>$B$14</f>
         <v>C</v>
       </c>
-      <c r="K6" s="51"/>
+      <c r="K6" s="30"/>
       <c r="L6" s="49" t="str">
         <f>B26</f>
         <v>UD + C</v>
@@ -1340,34 +1341,34 @@
     <row r="7" spans="1:15" ht="15.75" thickTop="1">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D7" s="41" t="str">
         <f>$B$14</f>
         <v>C</v>
       </c>
       <c r="E7" s="42"/>
-      <c r="F7" s="59" t="str">
+      <c r="F7" s="63" t="str">
         <f>$B$18</f>
         <v>X</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="59" t="str">
+      <c r="G7" s="64"/>
+      <c r="H7" s="28" t="str">
+        <f>B24</f>
+        <v>R + C</v>
+      </c>
+      <c r="I7" s="45" t="str">
+        <f>$B$21</f>
+        <v>-C</v>
+      </c>
+      <c r="J7" s="63" t="str">
         <f>$B$18</f>
         <v>X</v>
       </c>
-      <c r="I7" s="60"/>
-      <c r="J7" s="28" t="str">
-        <f>B24</f>
-        <v>R + C</v>
-      </c>
-      <c r="K7" s="45" t="str">
-        <f>$B$21</f>
-        <v>-C</v>
-      </c>
+      <c r="K7" s="64"/>
       <c r="L7" s="43" t="str">
         <f>B26</f>
         <v>UD + C</v>
@@ -1381,22 +1382,22 @@
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D8" s="47" t="str">
         <f>$B$14</f>
         <v>C</v>
       </c>
       <c r="E8" s="48"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="30" t="str">
+      <c r="F8" s="65"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="30" t="str">
         <f>$B$14</f>
         <v>C</v>
       </c>
-      <c r="K8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="66"/>
       <c r="L8" s="49" t="str">
         <f>B26</f>
         <v>UD + C</v>
@@ -1408,17 +1409,17 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" thickTop="1">
       <c r="A9" s="12"/>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="55" t="str">
+        <v>38</v>
+      </c>
+      <c r="D9" s="59" t="str">
         <f>$B$18</f>
         <v>X</v>
       </c>
-      <c r="E9" s="56"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="28" t="str">
         <f>$B$15</f>
         <v>R</v>
@@ -1428,32 +1429,32 @@
         <v>-A</v>
       </c>
       <c r="H9" s="28" t="str">
+        <f>$B$15</f>
+        <v>R</v>
+      </c>
+      <c r="I9" s="45" t="str">
+        <f>$B$21</f>
+        <v>-C</v>
+      </c>
+      <c r="J9" s="28" t="str">
         <f>$B$16</f>
         <v>A</v>
       </c>
-      <c r="I9" s="46" t="str">
+      <c r="K9" s="46" t="str">
         <f>$B$20</f>
         <v>-R</v>
       </c>
-      <c r="J9" s="28" t="str">
-        <f>$B$15</f>
-        <v>R</v>
-      </c>
-      <c r="K9" s="45" t="str">
-        <f>$B$21</f>
-        <v>-C</v>
-      </c>
-      <c r="L9" s="53" t="str">
+      <c r="L9" s="57" t="str">
         <f>$B$18</f>
         <v>X</v>
       </c>
-      <c r="M9" s="54"/>
+      <c r="M9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1">
       <c r="A10" s="12"/>
       <c r="B10" s="17"/>
       <c r="C10" s="15" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D10" s="47" t="str">
         <f>$B$14</f>
@@ -1487,83 +1488,83 @@
     <row r="11" spans="1:15" ht="15.75" thickTop="1"/>
     <row r="13" spans="1:15">
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="52"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="52"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="52" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" s="52"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21" s="52"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="52" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22" s="52"/>
     </row>
@@ -1603,11 +1604,11 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="J7:K8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -1618,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1629,8 +1630,8 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" customWidth="1"/>
   </cols>
@@ -1639,11 +1640,11 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="35">
-        <f>COUNTBLANK(F5:J28)</f>
+      <c r="G2" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="35">
+        <f>COUNTBLANK(E5:I28)</f>
         <v>104</v>
       </c>
     </row>
@@ -1653,37 +1654,37 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="12"/>
-      <c r="B5" s="63" t="s">
-        <v>16</v>
+      <c r="B5" s="53" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="str">
         <f>$K$5</f>
@@ -1695,12 +1696,12 @@
       <c r="H5" s="20"/>
       <c r="I5" s="21"/>
       <c r="K5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A6" s="12"/>
-      <c r="B6" s="64"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="14"/>
       <c r="D6" s="9" t="str">
         <f>$K$6</f>
@@ -1712,12 +1713,12 @@
       <c r="H6" s="3"/>
       <c r="I6" s="23"/>
       <c r="K6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A7" s="12"/>
-      <c r="B7" s="64"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="14"/>
       <c r="D7" s="9" t="str">
         <f>$K$7</f>
@@ -1729,12 +1730,12 @@
       <c r="H7" s="3"/>
       <c r="I7" s="23"/>
       <c r="K7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="12"/>
-      <c r="B8" s="64"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="16"/>
       <c r="D8" s="34" t="str">
         <f>$K$8</f>
@@ -1746,14 +1747,14 @@
       <c r="H8" s="11"/>
       <c r="I8" s="33"/>
       <c r="K8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" s="12"/>
-      <c r="B9" s="64"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="18" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8" t="str">
         <f>$K$5</f>
@@ -1767,7 +1768,7 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="64"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="14"/>
       <c r="D10" s="9" t="str">
         <f>$K$6</f>
@@ -1781,7 +1782,7 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A11" s="12"/>
-      <c r="B11" s="64"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="14"/>
       <c r="D11" s="9" t="str">
         <f>$K$7</f>
@@ -1795,7 +1796,7 @@
     </row>
     <row r="12" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A12" s="12"/>
-      <c r="B12" s="65"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="15"/>
       <c r="D12" s="9" t="str">
         <f>$K$8</f>
@@ -1810,10 +1811,10 @@
     <row r="13" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D13" s="9" t="str">
         <f>$K$5</f>
@@ -1821,12 +1822,12 @@
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1839,12 +1840,12 @@
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1857,12 +1858,12 @@
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
@@ -1875,19 +1876,19 @@
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="12"/>
       <c r="B17" s="14"/>
       <c r="C17" s="18" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D17" s="8" t="str">
         <f>$K$5</f>
@@ -1895,12 +1896,12 @@
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
@@ -1913,12 +1914,12 @@
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
@@ -1931,12 +1932,12 @@
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
@@ -1949,21 +1950,21 @@
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="25"/>
+        <v>16</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30" t="s">
+        <v>16</v>
+      </c>
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A21" s="12"/>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="56" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D21" s="9" t="str">
         <f>$K$5</f>
@@ -1977,7 +1978,7 @@
     </row>
     <row r="22" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="12"/>
-      <c r="B22" s="64"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="14"/>
       <c r="D22" s="9" t="str">
         <f>$K$6</f>
@@ -1991,7 +1992,7 @@
     </row>
     <row r="23" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A23" s="12"/>
-      <c r="B23" s="64"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="14"/>
       <c r="D23" s="9" t="str">
         <f>$K$7</f>
@@ -2005,7 +2006,7 @@
     </row>
     <row r="24" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A24" s="12"/>
-      <c r="B24" s="64"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="16"/>
       <c r="D24" s="34" t="str">
         <f>$K$8</f>
@@ -2019,9 +2020,9 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="12"/>
-      <c r="B25" s="64"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="18" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D25" s="8" t="str">
         <f>$K$5</f>
@@ -2035,7 +2036,7 @@
     </row>
     <row r="26" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A26" s="12"/>
-      <c r="B26" s="64"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="14"/>
       <c r="D26" s="9" t="str">
         <f>$K$6</f>
@@ -2049,7 +2050,7 @@
     </row>
     <row r="27" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A27" s="12"/>
-      <c r="B27" s="64"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="14"/>
       <c r="D27" s="9" t="str">
         <f>$K$7</f>

</xml_diff>